<commit_message>
add check script predict method of di series and check for DI4CompareImproveSelect and DI4NonStrategyImproveSelect
</commit_message>
<xml_diff>
--- a/co-scheduling/tmp/data.xlsx
+++ b/co-scheduling/tmp/data.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="24">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">Adaptive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &lt; B</t>
   </si>
   <si>
     <t xml:space="preserve">miss rate</t>
@@ -200,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -210,6 +213,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,7 +296,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -362,6 +369,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -569,11 +577,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="35664899"/>
-        <c:axId val="1939159"/>
+        <c:axId val="48238420"/>
+        <c:axId val="15723975"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35664899"/>
+        <c:axId val="48238420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,14 +617,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1939159"/>
+        <c:crossAx val="15723975"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1939159"/>
+        <c:axId val="15723975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +667,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35664899"/>
+        <c:crossAx val="48238420"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -698,9 +706,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -708,8 +716,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16348680" y="761760"/>
-        <a:ext cx="8647920" cy="2445840"/>
+        <a:off x="16367760" y="761760"/>
+        <a:ext cx="8657280" cy="2445480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -735,17 +743,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="9.36032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.36032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1416,16 +1425,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="9.36032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.36032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2096,16 +2106,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4898785425101"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1023" min="7" style="1" width="9.36032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.36032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1023" min="7" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2768,20 +2779,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="22.3036437246964"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.36032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2790,6 +2802,9 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,6 +2820,10 @@
       <c r="D2" s="1" t="n">
         <v>0.00548616104437322</v>
       </c>
+      <c r="E2" s="3" t="n">
+        <f aca="false">B2&lt;C2</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -2819,6 +2838,10 @@
       <c r="D3" s="1" t="n">
         <v>0.0077541726691698</v>
       </c>
+      <c r="E3" s="3" t="n">
+        <f aca="false">B3&lt;C3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -2833,6 +2856,10 @@
       <c r="D4" s="1" t="n">
         <v>0.0120998491267876</v>
       </c>
+      <c r="E4" s="3" t="n">
+        <f aca="false">B4&lt;C4</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -2847,6 +2874,10 @@
       <c r="D5" s="1" t="n">
         <v>0.00470806256133326</v>
       </c>
+      <c r="E5" s="3" t="n">
+        <f aca="false">B5&lt;C5</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -2861,6 +2892,10 @@
       <c r="D6" s="1" t="n">
         <v>0.00334520498475449</v>
       </c>
+      <c r="E6" s="3" t="n">
+        <f aca="false">B6&lt;C6</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -2875,6 +2910,10 @@
       <c r="D7" s="1" t="n">
         <v>4.68299982507231E-005</v>
       </c>
+      <c r="E7" s="3" t="n">
+        <f aca="false">B7&lt;C7</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -2889,6 +2928,10 @@
       <c r="D8" s="1" t="n">
         <v>0.00286057179471236</v>
       </c>
+      <c r="E8" s="3" t="n">
+        <f aca="false">B8&lt;C8</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -2903,6 +2946,10 @@
       <c r="D9" s="1" t="n">
         <v>0.000489028027673458</v>
       </c>
+      <c r="E9" s="3" t="n">
+        <f aca="false">B9&lt;C9</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -2917,6 +2964,10 @@
       <c r="D10" s="1" t="n">
         <v>7.09095965779766E-007</v>
       </c>
+      <c r="E10" s="3" t="n">
+        <f aca="false">B10&lt;C10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -2931,6 +2982,10 @@
       <c r="D11" s="1" t="n">
         <v>0.0117809552791999</v>
       </c>
+      <c r="E11" s="3" t="n">
+        <f aca="false">B11&lt;C11</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -2945,6 +3000,10 @@
       <c r="D12" s="1" t="n">
         <v>0.00225145980835913</v>
       </c>
+      <c r="E12" s="3" t="n">
+        <f aca="false">B12&lt;C12</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -2959,6 +3018,10 @@
       <c r="D13" s="1" t="n">
         <v>0.00401530337814999</v>
       </c>
+      <c r="E13" s="3" t="n">
+        <f aca="false">B13&lt;C13</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -2973,6 +3036,10 @@
       <c r="D14" s="1" t="n">
         <v>0.00942223261982817</v>
       </c>
+      <c r="E14" s="3" t="n">
+        <f aca="false">B14&lt;C14</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -2987,6 +3054,10 @@
       <c r="D15" s="1" t="n">
         <v>0.00424061977421474</v>
       </c>
+      <c r="E15" s="3" t="n">
+        <f aca="false">B15&lt;C15</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -3001,6 +3072,10 @@
       <c r="D16" s="1" t="n">
         <v>0.0220462711993997</v>
       </c>
+      <c r="E16" s="3" t="n">
+        <f aca="false">B16&lt;C16</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -3015,6 +3090,10 @@
       <c r="D17" s="1" t="n">
         <v>0.00477549099514854</v>
       </c>
+      <c r="E17" s="3" t="n">
+        <f aca="false">B17&lt;C17</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -3029,6 +3108,10 @@
       <c r="D18" s="1" t="n">
         <v>0.00414186724887502</v>
       </c>
+      <c r="E18" s="3" t="n">
+        <f aca="false">B18&lt;C18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -3043,6 +3126,10 @@
       <c r="D19" s="1" t="n">
         <v>0.00136370549483551</v>
       </c>
+      <c r="E19" s="3" t="n">
+        <f aca="false">B19&lt;C19</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -3057,6 +3144,10 @@
       <c r="D20" s="1" t="n">
         <v>0.00413647687397057</v>
       </c>
+      <c r="E20" s="3" t="n">
+        <f aca="false">B20&lt;C20</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -3071,6 +3162,10 @@
       <c r="D21" s="1" t="n">
         <v>0.000187944753129998</v>
       </c>
+      <c r="E21" s="3" t="n">
+        <f aca="false">B21&lt;C21</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -3085,6 +3180,10 @@
       <c r="D22" s="1" t="n">
         <v>0.0132059366631515</v>
       </c>
+      <c r="E22" s="3" t="n">
+        <f aca="false">B22&lt;C22</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -3099,6 +3198,10 @@
       <c r="D23" s="1" t="n">
         <v>0.000894319141377339</v>
       </c>
+      <c r="E23" s="3" t="n">
+        <f aca="false">B23&lt;C23</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -3113,6 +3216,10 @@
       <c r="D24" s="1" t="n">
         <v>0.000461900369450984</v>
       </c>
+      <c r="E24" s="3" t="n">
+        <f aca="false">B24&lt;C24</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -3127,6 +3234,10 @@
       <c r="D25" s="1" t="n">
         <v>0.000425738143413069</v>
       </c>
+      <c r="E25" s="3" t="n">
+        <f aca="false">B25&lt;C25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
@@ -3141,6 +3252,10 @@
       <c r="D26" s="1" t="n">
         <v>0.0159660121432097</v>
       </c>
+      <c r="E26" s="3" t="n">
+        <f aca="false">B26&lt;C26</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
@@ -3155,6 +3270,10 @@
       <c r="D27" s="1" t="n">
         <v>0.0193932089710198</v>
       </c>
+      <c r="E27" s="3" t="n">
+        <f aca="false">B27&lt;C27</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
@@ -3169,6 +3288,10 @@
       <c r="D28" s="1" t="n">
         <v>0.00892256395372521</v>
       </c>
+      <c r="E28" s="3" t="n">
+        <f aca="false">B28&lt;C28</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -3183,6 +3306,10 @@
       <c r="D29" s="1" t="n">
         <v>0.000243925488106657</v>
       </c>
+      <c r="E29" s="3" t="n">
+        <f aca="false">B29&lt;C29</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -3197,6 +3324,10 @@
       <c r="D30" s="1" t="n">
         <v>0.00985966080667349</v>
       </c>
+      <c r="E30" s="3" t="n">
+        <f aca="false">B30&lt;C30</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -3210,6 +3341,10 @@
       </c>
       <c r="D31" s="1" t="n">
         <v>0.00392931483852889</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <f aca="false">B31&lt;C31</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3236,18 +3371,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.6"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,27 +4971,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.6"/>
   <cols>
+    <col collapsed="false" hidden="false" max="9" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="Q1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6381,1576 +6520,1583 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="3" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="3" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="3" width="9"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="3" width="9"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="9"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="4" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="4" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="4" width="9"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="4" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="4" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="4" width="9"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="4" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="4" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="0"/>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>22</v>
+      <c r="P1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>20000076241</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>10539707117</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>1834559</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>43134113</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.042532</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>1.897593</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="3" t="n">
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4" t="n">
         <v>20000063884</v>
       </c>
-      <c r="K2" s="3" t="n">
+      <c r="K2" s="4" t="n">
         <v>10645216439</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="4" t="n">
         <v>2186205</v>
       </c>
-      <c r="M2" s="3" t="n">
+      <c r="M2" s="4" t="n">
         <v>42908945</v>
       </c>
-      <c r="N2" s="3" t="n">
+      <c r="N2" s="4" t="n">
         <v>0.05095</v>
       </c>
-      <c r="O2" s="3" t="n">
+      <c r="O2" s="4" t="n">
         <v>1.878784</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="n">
+      <c r="P2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="n">
         <f aca="false">D2-L2</f>
         <v>-351646</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>20000007096</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>48260219186</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>441640565</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>1381984267</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="4" t="n">
         <v>0.31957</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <v>0.41442</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="3" t="n">
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4" t="n">
         <v>20000003109</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="4" t="n">
         <v>47702895200</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <v>429000082</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <v>1380060300</v>
       </c>
-      <c r="N3" s="3" t="n">
+      <c r="N3" s="4" t="n">
         <v>0.310856</v>
       </c>
-      <c r="O3" s="3" t="n">
+      <c r="O3" s="4" t="n">
         <v>0.419262</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="3" t="n">
+      <c r="P3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="4" t="n">
         <f aca="false">D3-L3</f>
         <v>12640483</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>20000154288</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>9241925953</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>7226637</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>90686477</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.079688</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <v>2.164068</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="3" t="n">
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="4" t="n">
         <v>20000165248</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="4" t="n">
         <v>9711237206</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <v>11436709</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <v>90447056</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="4" t="n">
         <v>0.126446</v>
       </c>
-      <c r="O4" s="3" t="n">
+      <c r="O4" s="4" t="n">
         <v>2.059487</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="3" t="n">
+      <c r="P4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="4" t="n">
         <f aca="false">D4-L4</f>
         <v>-4210072</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>20000061919</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>20329416794</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>64250975</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>245867746</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.261323</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.983799</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="3" t="n">
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="4" t="n">
         <v>20000168654</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="4" t="n">
         <v>17771998941</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <v>41454534</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="4" t="n">
         <v>245821202</v>
       </c>
-      <c r="N5" s="3" t="n">
+      <c r="N5" s="4" t="n">
         <v>0.168637</v>
       </c>
-      <c r="O5" s="3" t="n">
+      <c r="O5" s="4" t="n">
         <v>1.125375</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R5" s="3" t="n">
+      <c r="P5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5" s="4" t="n">
         <f aca="false">D5-L5</f>
         <v>22796441</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>20000055095</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>27930509499</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>330574450</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>617020453</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.535759</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>0.716065</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="n">
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="4" t="n">
         <v>20000049100</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <v>31067255658</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <v>590131017</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <v>665023427</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="4" t="n">
         <v>0.887384</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="O6" s="4" t="n">
         <v>0.643766</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" s="3" t="n">
+      <c r="P6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="4" t="n">
         <f aca="false">D6-L6</f>
         <v>-259556567</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>20000073651</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>29334998096</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>633193673</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>634531493</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>0.997892</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <v>0.681782</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="3" t="n">
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
         <v>20000076538</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="4" t="n">
         <v>27097176250</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="4" t="n">
         <v>520815552</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="4" t="n">
         <v>634530076</v>
       </c>
-      <c r="N7" s="3" t="n">
+      <c r="N7" s="4" t="n">
         <v>0.820789</v>
       </c>
-      <c r="O7" s="3" t="n">
+      <c r="O7" s="4" t="n">
         <v>0.738087</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="3" t="n">
+      <c r="P7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="4" t="n">
         <f aca="false">D7-L7</f>
         <v>112378121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>19999974803</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>56959796548</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>571073297</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>621197797</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>0.91931</v>
       </c>
-      <c r="G8" s="3" t="n">
+      <c r="G8" s="4" t="n">
         <v>0.351124</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="3" t="n">
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="4" t="n">
         <v>20000005741</v>
       </c>
-      <c r="K8" s="3" t="n">
+      <c r="K8" s="4" t="n">
         <v>56763725611</v>
       </c>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="4" t="n">
         <v>549914111</v>
       </c>
-      <c r="M8" s="3" t="n">
+      <c r="M8" s="4" t="n">
         <v>621592688</v>
       </c>
-      <c r="N8" s="3" t="n">
+      <c r="N8" s="4" t="n">
         <v>0.884686</v>
       </c>
-      <c r="O8" s="3" t="n">
+      <c r="O8" s="4" t="n">
         <v>0.352338</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R8" s="3" t="n">
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="4" t="n">
         <f aca="false">D8-L8</f>
         <v>21159186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="4" t="n">
         <v>20000033383</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>13615936618</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>8226145</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>482595290</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <v>0.017046</v>
       </c>
-      <c r="G9" s="3" t="n">
+      <c r="G9" s="4" t="n">
         <v>1.468869</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="3" t="n">
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="4" t="n">
         <v>20000113884</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="K9" s="4" t="n">
         <v>13149928118</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="4" t="n">
         <v>6755044</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="4" t="n">
         <v>482758664</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="4" t="n">
         <v>0.013993</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="4" t="n">
         <v>1.52093</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="3" t="n">
+      <c r="P9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" s="4" t="n">
         <f aca="false">D9-L9</f>
         <v>1471101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>20000102154</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>9869139912</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>4041660</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>66179902</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <v>0.061071</v>
       </c>
-      <c r="G10" s="3" t="n">
+      <c r="G10" s="4" t="n">
         <v>2.026529</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="3" t="n">
+      <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="4" t="n">
         <v>20000089855</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="4" t="n">
         <v>9820118200</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <v>3710494</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <v>65724085</v>
       </c>
-      <c r="N10" s="3" t="n">
+      <c r="N10" s="4" t="n">
         <v>0.056456</v>
       </c>
-      <c r="O10" s="3" t="n">
+      <c r="O10" s="4" t="n">
         <v>2.036645</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R10" s="3" t="n">
+      <c r="P10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="4" t="n">
         <f aca="false">D10-L10</f>
         <v>331166</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="4" t="n">
         <v>502</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>19999987835</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>35712592057</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>193890985</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>342606257</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="4" t="n">
         <v>0.565929</v>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="4" t="n">
         <v>0.560026</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="3" t="n">
+      <c r="H11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="4" t="n">
         <v>19999976610</v>
       </c>
-      <c r="K11" s="3" t="n">
+      <c r="K11" s="4" t="n">
         <v>35545298693</v>
       </c>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="4" t="n">
         <v>197596850</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <v>343858713</v>
       </c>
-      <c r="N11" s="3" t="n">
+      <c r="N11" s="4" t="n">
         <v>0.574645</v>
       </c>
-      <c r="O11" s="3" t="n">
+      <c r="O11" s="4" t="n">
         <v>0.562662</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R11" s="3" t="n">
+      <c r="P11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="4" t="n">
         <f aca="false">D11-L11</f>
         <v>-3705865</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="4" t="n">
         <v>505</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>19999988569</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>30389541622</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>235194163</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <v>592836140</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="4" t="n">
         <v>0.396727</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="4" t="n">
         <v>0.658121</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="3" t="n">
+      <c r="H12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="4" t="n">
         <v>20000002601</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="4" t="n">
         <v>31694476144</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="4" t="n">
         <v>248034091</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <v>594548235</v>
       </c>
-      <c r="N12" s="3" t="n">
+      <c r="N12" s="4" t="n">
         <v>0.417181</v>
       </c>
-      <c r="O12" s="3" t="n">
+      <c r="O12" s="4" t="n">
         <v>0.631025</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R12" s="3" t="n">
+      <c r="P12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="4" t="n">
         <f aca="false">D12-L12</f>
         <v>-12839928</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="4" t="n">
         <v>519</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>19999991603</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>25710583347</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>304754971</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="4" t="n">
         <v>553303391</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="4" t="n">
         <v>0.550792</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="4" t="n">
         <v>0.777889</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="3" t="n">
+      <c r="H13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="4" t="n">
         <v>19999995273</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="4" t="n">
         <v>27820990607</v>
       </c>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="4" t="n">
         <v>528245978</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="4" t="n">
         <v>605432986</v>
       </c>
-      <c r="N13" s="3" t="n">
+      <c r="N13" s="4" t="n">
         <v>0.872509</v>
       </c>
-      <c r="O13" s="3" t="n">
+      <c r="O13" s="4" t="n">
         <v>0.718881</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="3" t="n">
+      <c r="P13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="4" t="n">
         <f aca="false">D13-L13</f>
         <v>-223491007</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="4" t="n">
         <v>520</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>20000001088</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="4" t="n">
         <v>34650419230</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>163044919</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="4" t="n">
         <v>433191821</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="4" t="n">
         <v>0.37638</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="4" t="n">
         <v>0.577194</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="3" t="n">
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="4" t="n">
         <v>19999999898</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="4" t="n">
         <v>35621931689</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="4" t="n">
         <v>175639006</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <v>433740571</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="4" t="n">
         <v>0.40494</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="4" t="n">
         <v>0.561452</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R14" s="3" t="n">
+      <c r="P14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" s="4" t="n">
         <f aca="false">D14-L14</f>
         <v>-12594087</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="4" t="n">
         <v>521</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>20000091397</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="4" t="n">
         <v>20029202827</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="4" t="n">
         <v>66791397</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="4" t="n">
         <v>138730776</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="4" t="n">
         <v>0.481446</v>
       </c>
-      <c r="G15" s="3" t="n">
+      <c r="G15" s="4" t="n">
         <v>0.998547</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="3" t="n">
+      <c r="H15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="4" t="n">
         <v>20000066079</v>
       </c>
-      <c r="K15" s="3" t="n">
+      <c r="K15" s="4" t="n">
         <v>21398911946</v>
       </c>
-      <c r="L15" s="3" t="n">
+      <c r="L15" s="4" t="n">
         <v>78971048</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="M15" s="4" t="n">
         <v>145011544</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="N15" s="4" t="n">
         <v>0.544585</v>
       </c>
-      <c r="O15" s="3" t="n">
+      <c r="O15" s="4" t="n">
         <v>0.93463</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R15" s="3" t="n">
+      <c r="P15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" s="4" t="n">
         <f aca="false">D15-L15</f>
         <v>-12179651</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="4" t="n">
         <v>523</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>20000003142</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="4" t="n">
         <v>15775742949</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="4" t="n">
         <v>11907543</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="4" t="n">
         <v>601263864</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="4" t="n">
         <v>0.019804</v>
       </c>
-      <c r="G16" s="3" t="n">
+      <c r="G16" s="4" t="n">
         <v>1.267769</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="3" t="n">
+      <c r="H16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="4" t="n">
         <v>19999998323</v>
       </c>
-      <c r="K16" s="3" t="n">
+      <c r="K16" s="4" t="n">
         <v>15342771148</v>
       </c>
-      <c r="L16" s="3" t="n">
+      <c r="L16" s="4" t="n">
         <v>8806685</v>
       </c>
-      <c r="M16" s="3" t="n">
+      <c r="M16" s="4" t="n">
         <v>601284226</v>
       </c>
-      <c r="N16" s="3" t="n">
+      <c r="N16" s="4" t="n">
         <v>0.014646</v>
       </c>
-      <c r="O16" s="3" t="n">
+      <c r="O16" s="4" t="n">
         <v>1.303545</v>
       </c>
-      <c r="P16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R16" s="3" t="n">
+      <c r="P16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" s="4" t="n">
         <f aca="false">D16-L16</f>
         <v>3100858</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="4" t="n">
         <v>544</v>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>19999995688</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="4" t="n">
         <v>17949970368</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="4" t="n">
         <v>8937078</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="4" t="n">
         <v>16315239</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="4" t="n">
         <v>0.547775</v>
       </c>
-      <c r="G17" s="3" t="n">
+      <c r="G17" s="4" t="n">
         <v>1.114208</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="3" t="n">
+      <c r="H17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="4" t="n">
         <v>19999986772</v>
       </c>
-      <c r="K17" s="3" t="n">
+      <c r="K17" s="4" t="n">
         <v>18138214051</v>
       </c>
-      <c r="L17" s="3" t="n">
+      <c r="L17" s="4" t="n">
         <v>9164753</v>
       </c>
-      <c r="M17" s="3" t="n">
+      <c r="M17" s="4" t="n">
         <v>40381020</v>
       </c>
-      <c r="N17" s="3" t="n">
+      <c r="N17" s="4" t="n">
         <v>0.226957</v>
       </c>
-      <c r="O17" s="3" t="n">
+      <c r="O17" s="4" t="n">
         <v>1.102644</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R17" s="3" t="n">
+      <c r="P17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R17" s="4" t="n">
         <f aca="false">D17-L17</f>
         <v>-227675</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="4" t="n">
         <v>548</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>19999993490</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="4" t="n">
         <v>8474454664</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="4" t="n">
         <v>970</v>
       </c>
-      <c r="E18" s="3" t="n">
+      <c r="E18" s="4" t="n">
         <v>10425</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="4" t="n">
         <v>0.093046</v>
       </c>
-      <c r="G18" s="3" t="n">
+      <c r="G18" s="4" t="n">
         <v>2.360033</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="3" t="n">
+      <c r="H18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="4" t="n">
         <v>19999995405</v>
       </c>
-      <c r="K18" s="3" t="n">
+      <c r="K18" s="4" t="n">
         <v>8466892250</v>
       </c>
-      <c r="L18" s="3" t="n">
+      <c r="L18" s="4" t="n">
         <v>8384</v>
       </c>
-      <c r="M18" s="3" t="n">
+      <c r="M18" s="4" t="n">
         <v>53935</v>
       </c>
-      <c r="N18" s="3" t="n">
+      <c r="N18" s="4" t="n">
         <v>0.155446</v>
       </c>
-      <c r="O18" s="3" t="n">
+      <c r="O18" s="4" t="n">
         <v>2.362141</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R18" s="3" t="n">
+      <c r="P18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R18" s="4" t="n">
         <f aca="false">D18-L18</f>
         <v>-7414</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="4" t="n">
         <v>549</v>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>19999989239</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="4" t="n">
         <v>41384315648</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="4" t="n">
         <v>482584477</v>
       </c>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="4" t="n">
         <v>588415766</v>
       </c>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="4" t="n">
         <v>0.820142</v>
       </c>
-      <c r="G19" s="3" t="n">
+      <c r="G19" s="4" t="n">
         <v>0.483275</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="3" t="n">
+      <c r="H19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="4" t="n">
         <v>19999986402</v>
       </c>
-      <c r="K19" s="3" t="n">
+      <c r="K19" s="4" t="n">
         <v>44617501375</v>
       </c>
-      <c r="L19" s="3" t="n">
+      <c r="L19" s="4" t="n">
         <v>571789455</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="M19" s="4" t="n">
         <v>593358824</v>
       </c>
-      <c r="N19" s="3" t="n">
+      <c r="N19" s="4" t="n">
         <v>0.963649</v>
       </c>
-      <c r="O19" s="3" t="n">
+      <c r="O19" s="4" t="n">
         <v>0.448254</v>
       </c>
-      <c r="P19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R19" s="3" t="n">
+      <c r="P19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" s="4" t="n">
         <f aca="false">D19-L19</f>
         <v>-89204978</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="4" t="n">
         <v>557</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>19999992683</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="4" t="n">
         <v>29221617322</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="4" t="n">
         <v>71875397</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="4" t="n">
         <v>193961779</v>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>0.370565</v>
       </c>
-      <c r="G20" s="3" t="n">
+      <c r="G20" s="4" t="n">
         <v>0.684425</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="3" t="n">
+      <c r="H20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="4" t="n">
         <v>19999980536</v>
       </c>
-      <c r="K20" s="3" t="n">
+      <c r="K20" s="4" t="n">
         <v>28160669752</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="4" t="n">
         <v>63676098</v>
       </c>
-      <c r="M20" s="3" t="n">
+      <c r="M20" s="4" t="n">
         <v>192514848</v>
       </c>
-      <c r="N20" s="3" t="n">
+      <c r="N20" s="4" t="n">
         <v>0.330759</v>
       </c>
-      <c r="O20" s="3" t="n">
+      <c r="O20" s="4" t="n">
         <v>0.71021</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R20" s="3" t="n">
+      <c r="P20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R20" s="4" t="n">
         <f aca="false">D20-L20</f>
         <v>8199299</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="4" t="n">
         <v>602</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>20000011028</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="4" t="n">
         <v>114913943978</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="4" t="n">
         <v>538009019</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="4" t="n">
         <v>554724199</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="4" t="n">
         <v>0.969868</v>
       </c>
-      <c r="G21" s="3" t="n">
+      <c r="G21" s="4" t="n">
         <v>0.174043</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="3" t="n">
+      <c r="H21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="4" t="n">
         <v>20000008804</v>
       </c>
-      <c r="K21" s="3" t="n">
+      <c r="K21" s="4" t="n">
         <v>85483261573</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="L21" s="4" t="n">
         <v>338597129</v>
       </c>
-      <c r="M21" s="3" t="n">
+      <c r="M21" s="4" t="n">
         <v>554150286</v>
       </c>
-      <c r="N21" s="3" t="n">
+      <c r="N21" s="4" t="n">
         <v>0.61102</v>
       </c>
-      <c r="O21" s="3" t="n">
+      <c r="O21" s="4" t="n">
         <v>0.233964</v>
       </c>
-      <c r="P21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R21" s="3" t="n">
+      <c r="P21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R21" s="4" t="n">
         <f aca="false">D21-L21</f>
         <v>199411890</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="4" t="n">
         <v>605</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>20000007882</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="4" t="n">
         <v>38975499278</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="4" t="n">
         <v>442755865</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="4" t="n">
         <v>1126918995</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>0.392891</v>
       </c>
-      <c r="G22" s="3" t="n">
+      <c r="G22" s="4" t="n">
         <v>0.513143</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="3" t="n">
+      <c r="H22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="4" t="n">
         <v>20000036245</v>
       </c>
-      <c r="K22" s="3" t="n">
+      <c r="K22" s="4" t="n">
         <v>36629292294</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="4" t="n">
         <v>348210661</v>
       </c>
-      <c r="M22" s="3" t="n">
+      <c r="M22" s="4" t="n">
         <v>1125187805</v>
       </c>
-      <c r="N22" s="3" t="n">
+      <c r="N22" s="4" t="n">
         <v>0.309469</v>
       </c>
-      <c r="O22" s="3" t="n">
+      <c r="O22" s="4" t="n">
         <v>0.546012</v>
       </c>
-      <c r="P22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R22" s="3" t="n">
+      <c r="P22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" s="4" t="n">
         <f aca="false">D22-L22</f>
         <v>94545204</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="4" t="n">
         <v>607</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="4" t="n">
         <v>20000027594</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="4" t="n">
         <v>21234482563</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="4" t="n">
         <v>90209599</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="4" t="n">
         <v>264913242</v>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="4" t="n">
         <v>0.340525</v>
       </c>
-      <c r="G23" s="3" t="n">
+      <c r="G23" s="4" t="n">
         <v>0.941866</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="3" t="n">
+      <c r="H23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="4" t="n">
         <v>20000009460</v>
       </c>
-      <c r="K23" s="3" t="n">
+      <c r="K23" s="4" t="n">
         <v>22423797958</v>
       </c>
-      <c r="L23" s="3" t="n">
+      <c r="L23" s="4" t="n">
         <v>99564400</v>
       </c>
-      <c r="M23" s="3" t="n">
+      <c r="M23" s="4" t="n">
         <v>262943871</v>
       </c>
-      <c r="N23" s="3" t="n">
+      <c r="N23" s="4" t="n">
         <v>0.378653</v>
       </c>
-      <c r="O23" s="3" t="n">
+      <c r="O23" s="4" t="n">
         <v>0.89191</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R23" s="3" t="n">
+      <c r="P23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="4" t="n">
         <f aca="false">D23-L23</f>
         <v>-9354801</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="4" t="n">
         <v>619</v>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="4" t="n">
         <v>20000006881</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="4" t="n">
         <v>29913060865</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="4" t="n">
         <v>663170288</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="4" t="n">
         <v>764269325</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="4" t="n">
         <v>0.867718</v>
       </c>
-      <c r="G24" s="3" t="n">
+      <c r="G24" s="4" t="n">
         <v>0.668604</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="3" t="n">
+      <c r="H24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="4" t="n">
         <v>20000018935</v>
       </c>
-      <c r="K24" s="3" t="n">
+      <c r="K24" s="4" t="n">
         <v>30137248149</v>
       </c>
-      <c r="L24" s="3" t="n">
+      <c r="L24" s="4" t="n">
         <v>680073331</v>
       </c>
-      <c r="M24" s="3" t="n">
+      <c r="M24" s="4" t="n">
         <v>798946350</v>
       </c>
-      <c r="N24" s="3" t="n">
+      <c r="N24" s="4" t="n">
         <v>0.851213</v>
       </c>
-      <c r="O24" s="3" t="n">
+      <c r="O24" s="4" t="n">
         <v>0.663631</v>
       </c>
-      <c r="P24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R24" s="3" t="n">
+      <c r="P24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R24" s="4" t="n">
         <f aca="false">D24-L24</f>
         <v>-16903043</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="4" t="n">
         <v>620</v>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="4" t="n">
         <v>20000005042</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="4" t="n">
         <v>34962436135</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="4" t="n">
         <v>163483075</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="4" t="n">
         <v>431938758</v>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="4" t="n">
         <v>0.378487</v>
       </c>
-      <c r="G25" s="3" t="n">
+      <c r="G25" s="4" t="n">
         <v>0.572043</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="3" t="n">
+      <c r="H25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="4" t="n">
         <v>19999988244</v>
       </c>
-      <c r="K25" s="3" t="n">
+      <c r="K25" s="4" t="n">
         <v>35600006036</v>
       </c>
-      <c r="L25" s="3" t="n">
+      <c r="L25" s="4" t="n">
         <v>174428855</v>
       </c>
-      <c r="M25" s="3" t="n">
+      <c r="M25" s="4" t="n">
         <v>432581570</v>
       </c>
-      <c r="N25" s="3" t="n">
+      <c r="N25" s="4" t="n">
         <v>0.403228</v>
       </c>
-      <c r="O25" s="3" t="n">
+      <c r="O25" s="4" t="n">
         <v>0.561797</v>
       </c>
-      <c r="P25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R25" s="3" t="n">
+      <c r="P25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R25" s="4" t="n">
         <f aca="false">D25-L25</f>
         <v>-10945780</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="4" t="n">
         <v>623</v>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>20000075089</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="4" t="n">
         <v>50517372831</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="4" t="n">
         <v>252830759</v>
       </c>
-      <c r="E26" s="3" t="n">
+      <c r="E26" s="4" t="n">
         <v>669686908</v>
       </c>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="4" t="n">
         <v>0.377536</v>
       </c>
-      <c r="G26" s="3" t="n">
+      <c r="G26" s="4" t="n">
         <v>0.395905</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="3" t="n">
+      <c r="H26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="4" t="n">
         <v>20000065350</v>
       </c>
-      <c r="K26" s="3" t="n">
+      <c r="K26" s="4" t="n">
         <v>39192643751</v>
       </c>
-      <c r="L26" s="3" t="n">
+      <c r="L26" s="4" t="n">
         <v>153270414</v>
       </c>
-      <c r="M26" s="3" t="n">
+      <c r="M26" s="4" t="n">
         <v>669436626</v>
       </c>
-      <c r="N26" s="3" t="n">
+      <c r="N26" s="4" t="n">
         <v>0.228954</v>
       </c>
-      <c r="O26" s="3" t="n">
+      <c r="O26" s="4" t="n">
         <v>0.510302</v>
       </c>
-      <c r="P26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R26" s="3" t="n">
+      <c r="P26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R26" s="4" t="n">
         <f aca="false">D26-L26</f>
         <v>99560345</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="4" t="n">
         <v>625</v>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="4" t="n">
         <v>20000069683</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="4" t="n">
         <v>7228200161</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="4" t="n">
         <v>9711686</v>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="E27" s="4" t="n">
         <v>17772993</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="4" t="n">
         <v>0.546429</v>
       </c>
-      <c r="G27" s="3" t="n">
+      <c r="G27" s="4" t="n">
         <v>2.76695</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="3" t="n">
+      <c r="H27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="4" t="n">
         <v>19999990260</v>
       </c>
-      <c r="K27" s="3" t="n">
+      <c r="K27" s="4" t="n">
         <v>7591256700</v>
       </c>
-      <c r="L27" s="3" t="n">
+      <c r="L27" s="4" t="n">
         <v>12365399</v>
       </c>
-      <c r="M27" s="3" t="n">
+      <c r="M27" s="4" t="n">
         <v>18065035</v>
       </c>
-      <c r="N27" s="3" t="n">
+      <c r="N27" s="4" t="n">
         <v>0.684493</v>
       </c>
-      <c r="O27" s="3" t="n">
+      <c r="O27" s="4" t="n">
         <v>2.634609</v>
       </c>
-      <c r="P27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R27" s="3" t="n">
+      <c r="P27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R27" s="4" t="n">
         <f aca="false">D27-L27</f>
         <v>-2653713</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="4" t="n">
         <v>627</v>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="4" t="n">
         <v>9999922347</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="4" t="n">
         <v>6781659307</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="4" t="n">
         <v>28123529</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="E28" s="4" t="n">
         <v>112034668</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="4" t="n">
         <v>0.251025</v>
       </c>
-      <c r="G28" s="3" t="n">
+      <c r="G28" s="4" t="n">
         <v>1.474554</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="3" t="n">
+      <c r="H28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="4" t="n">
         <v>9999858275</v>
       </c>
-      <c r="K28" s="3" t="n">
+      <c r="K28" s="4" t="n">
         <v>7198890892</v>
       </c>
-      <c r="L28" s="3" t="n">
+      <c r="L28" s="4" t="n">
         <v>33480256</v>
       </c>
-      <c r="M28" s="3" t="n">
+      <c r="M28" s="4" t="n">
         <v>116921660</v>
       </c>
-      <c r="N28" s="3" t="n">
+      <c r="N28" s="4" t="n">
         <v>0.286348</v>
       </c>
-      <c r="O28" s="3" t="n">
+      <c r="O28" s="4" t="n">
         <v>1.389083</v>
       </c>
-      <c r="P28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R28" s="3" t="n">
+      <c r="P28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R28" s="4" t="n">
         <f aca="false">D28-L28</f>
         <v>-5356727</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="4" t="n">
         <v>638</v>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="4" t="n">
         <v>20000000048</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="4" t="n">
         <v>10201574636</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="4" t="n">
         <v>2997775</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="4" t="n">
         <v>58945693</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="4" t="n">
         <v>0.050857</v>
       </c>
-      <c r="G29" s="3" t="n">
+      <c r="G29" s="4" t="n">
         <v>1.960482</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="3" t="n">
+      <c r="H29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="4" t="n">
         <v>20000019916</v>
       </c>
-      <c r="K29" s="3" t="n">
+      <c r="K29" s="4" t="n">
         <v>11604326072</v>
       </c>
-      <c r="L29" s="3" t="n">
+      <c r="L29" s="4" t="n">
         <v>9271891</v>
       </c>
-      <c r="M29" s="3" t="n">
+      <c r="M29" s="4" t="n">
         <v>54156936</v>
       </c>
-      <c r="N29" s="3" t="n">
+      <c r="N29" s="4" t="n">
         <v>0.171204</v>
       </c>
-      <c r="O29" s="3" t="n">
+      <c r="O29" s="4" t="n">
         <v>1.723497</v>
       </c>
-      <c r="P29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R29" s="3" t="n">
+      <c r="P29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R29" s="4" t="n">
         <f aca="false">D29-L29</f>
         <v>-6274116</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="4" t="n">
         <v>527</v>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="4" t="n">
         <v>19999946855</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="4" t="n">
         <v>14284924438</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="4" t="n">
         <v>42744931</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="4" t="n">
         <v>175994954</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="4" t="n">
         <v>0.242876</v>
       </c>
-      <c r="G30" s="3" t="n">
+      <c r="G30" s="4" t="n">
         <v>1.400074</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="3" t="n">
+      <c r="H30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="4" t="n">
         <v>19999976834</v>
       </c>
-      <c r="K30" s="3" t="n">
+      <c r="K30" s="4" t="n">
         <v>14371253643</v>
       </c>
-      <c r="L30" s="3" t="n">
+      <c r="L30" s="4" t="n">
         <v>46331844</v>
       </c>
-      <c r="M30" s="3" t="n">
+      <c r="M30" s="4" t="n">
         <v>172710102</v>
       </c>
-      <c r="N30" s="3" t="n">
+      <c r="N30" s="4" t="n">
         <v>0.268264</v>
       </c>
-      <c r="O30" s="3" t="n">
+      <c r="O30" s="4" t="n">
         <v>1.391665</v>
       </c>
-      <c r="P30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R30" s="3" t="n">
+      <c r="P30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" s="4" t="n">
         <f aca="false">D30-L30</f>
         <v>-3586913</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="4" t="n">
         <v>649</v>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="4" t="n">
         <v>20000029500</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="4" t="n">
         <v>42752907807</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="4" t="n">
         <v>559545705</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="4" t="n">
         <v>658891670</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>0.849223</v>
       </c>
-      <c r="G31" s="3" t="n">
+      <c r="G31" s="4" t="n">
         <v>0.467805</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="3" t="n">
+      <c r="H31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="4" t="n">
         <v>20000031503</v>
       </c>
-      <c r="K31" s="3" t="n">
+      <c r="K31" s="4" t="n">
         <v>42691102144</v>
       </c>
-      <c r="L31" s="3" t="n">
+      <c r="L31" s="4" t="n">
         <v>564733584</v>
       </c>
-      <c r="M31" s="3" t="n">
+      <c r="M31" s="4" t="n">
         <v>657497875</v>
       </c>
-      <c r="N31" s="3" t="n">
+      <c r="N31" s="4" t="n">
         <v>0.858913</v>
       </c>
-      <c r="O31" s="3" t="n">
+      <c r="O31" s="4" t="n">
         <v>0.468482</v>
       </c>
-      <c r="P31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R31" s="3" t="n">
+      <c r="P31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31" s="4" t="n">
         <f aca="false">D31-L31</f>
         <v>-5187879</v>
       </c>

</xml_diff>